<commit_message>
added possibility to change UID
</commit_message>
<xml_diff>
--- a/prince_archiver/entrypoints/mock_prince/2025_DataMigration.xlsx
+++ b/prince_archiver/entrypoints/mock_prince/2025_DataMigration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coren\AMOLF-SHIMIZU Dropbox\Corentin Bisot\AMF-PlateList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071B7D18-D402-4C8D-95D7-DFD96E869ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999CA43F-5AFA-4734-A00C-C6FCFF7F3538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,14 +557,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>